<commit_message>
more work done on project
</commit_message>
<xml_diff>
--- a/ptResultData.xlsx
+++ b/ptResultData.xlsx
@@ -257,7 +257,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -286,6 +286,7 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -590,7 +591,7 @@
   <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1043,10 +1044,23 @@
         <v>62</v>
       </c>
     </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="3"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+    </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>48</v>
       </c>
+      <c r="B22" s="10">
+        <v>5.2831000000000001</v>
+      </c>
       <c r="C22" s="11">
         <v>2.7519999999999998</v>
       </c>
@@ -1070,6 +1084,10 @@
       <c r="A23" s="12" t="s">
         <v>49</v>
       </c>
+      <c r="B23" s="14">
+        <f>B22/24</f>
+        <v>0.22012916666666668</v>
+      </c>
       <c r="C23" s="13">
         <f>C22/31</f>
         <v>8.8774193548387087E-2</v>
@@ -1097,6 +1115,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>